<commit_message>
Mise à jour du fichier HTML et du style
</commit_message>
<xml_diff>
--- a/Résultat_Test.xlsx
+++ b/Résultat_Test.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
@@ -507,6 +507,212 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>elisabeth venchiarutti</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>hello again</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Victoire</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Victoire</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Le grand succès</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Marc Clément </t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Elisabeth jeudi 15 aout</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>hourr ahourra</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Nathalie Marcot</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Nouvelle version</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>cest moi</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>